<commit_message>
small fix of labels on graphs
</commit_message>
<xml_diff>
--- a/Day4/Rwanda_visualizations.xlsx
+++ b/Day4/Rwanda_visualizations.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19380" windowHeight="6060" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19380" windowHeight="6060"/>
   </bookViews>
   <sheets>
     <sheet name="data+basic_plots" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="sparklines" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlcn.WorksheetConnection_Sheet5B3N6" hidden="1">sparklines!$B$3:$N$6</definedName>
+    <definedName name="_xlcn.WorksheetConnection_Sheet5B3N61" hidden="1">sparklines!$B$3:$N$6</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -52,7 +52,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="Range-7b0e4736-3173-42b0-9f06-e43d478a21cb" autoDelete="1" usedByAddin="1">
-          <x15:rangePr sourceName="_xlcn.WorksheetConnection_Sheet5B3N6"/>
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_Sheet5B3N61"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -6548,7 +6548,7 @@
                   <a:p>
                     <a:r>
                       <a:rPr lang="en-US"/>
-                      <a:t>0.20 B</a:t>
+                      <a:t>0.28 B</a:t>
                     </a:r>
                   </a:p>
                 </c:rich>
@@ -7086,7 +7086,7 @@
                   <a:p>
                     <a:r>
                       <a:rPr lang="en-US"/>
-                      <a:t>0.30 B</a:t>
+                      <a:t>0.33 B</a:t>
                     </a:r>
                   </a:p>
                 </c:rich>
@@ -16036,8 +16036,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="5572845" y="5053533"/>
-          <a:ext cx="6059510" cy="4678297"/>
+          <a:off x="5547808" y="5050267"/>
+          <a:ext cx="6033384" cy="4678297"/>
           <a:chOff x="5547808" y="5050267"/>
           <a:chExt cx="6033384" cy="4678297"/>
         </a:xfrm>
@@ -16198,8 +16198,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="7777322" y="238908"/>
-          <a:ext cx="6059509" cy="4684701"/>
+          <a:off x="7743576" y="238908"/>
+          <a:ext cx="6033384" cy="4681435"/>
           <a:chOff x="7255896" y="238908"/>
           <a:chExt cx="6033384" cy="4681435"/>
         </a:xfrm>
@@ -19931,8 +19931,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L178"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M10" sqref="M9:M10"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AG10" sqref="AG10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.25"/>
@@ -22194,7 +22194,31 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-        <x14:sparklineGroup displayEmptyCellsAs="gap" first="1" last="1">
+        <x14:sparklineGroup displayEmptyCellsAs="gap" high="1" first="1" last="1">
+          <x14:colorSeries theme="1" tint="0.499984740745262"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst theme="0" tint="-0.34998626667073579"/>
+          <x14:colorLast theme="0" tint="-0.499984740745262"/>
+          <x14:colorHigh rgb="FF00B050"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:sqref>C35</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:sqref>C36</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:sqref>C37</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:sqref>C38</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup displayEmptyCellsAs="gap" first="1" last="1" minAxisType="group">
           <x14:colorSeries theme="1" tint="0.499984740745262"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -22205,13 +22229,16 @@
           <x14:colorLow rgb="FFD00000"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:sqref>C31</xm:sqref>
+              <xm:f>heatmap!D7:Q7</xm:f>
+              <xm:sqref>R7</xm:sqref>
             </x14:sparkline>
             <x14:sparkline>
-              <xm:sqref>C32</xm:sqref>
+              <xm:f>heatmap!D8:Q8</xm:f>
+              <xm:sqref>R8</xm:sqref>
             </x14:sparkline>
             <x14:sparkline>
-              <xm:sqref>C33</xm:sqref>
+              <xm:f>heatmap!D9:Q9</xm:f>
+              <xm:sqref>R9</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
@@ -22243,7 +22270,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="gap" first="1" last="1" minAxisType="group">
+        <x14:sparklineGroup displayEmptyCellsAs="gap" first="1" last="1">
           <x14:colorSeries theme="1" tint="0.499984740745262"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -22254,40 +22281,13 @@
           <x14:colorLow rgb="FFD00000"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>heatmap!D7:Q7</xm:f>
-              <xm:sqref>R7</xm:sqref>
+              <xm:sqref>C31</xm:sqref>
             </x14:sparkline>
             <x14:sparkline>
-              <xm:f>heatmap!D8:Q8</xm:f>
-              <xm:sqref>R8</xm:sqref>
+              <xm:sqref>C32</xm:sqref>
             </x14:sparkline>
             <x14:sparkline>
-              <xm:f>heatmap!D9:Q9</xm:f>
-              <xm:sqref>R9</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="gap" high="1" first="1" last="1">
-          <x14:colorSeries theme="1" tint="0.499984740745262"/>
-          <x14:colorNegative rgb="FFD00000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst theme="0" tint="-0.34998626667073579"/>
-          <x14:colorLast theme="0" tint="-0.499984740745262"/>
-          <x14:colorHigh rgb="FF00B050"/>
-          <x14:colorLow rgb="FFD00000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:sqref>C35</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:sqref>C36</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:sqref>C37</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:sqref>C38</xm:sqref>
+              <xm:sqref>C33</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
@@ -22301,7 +22301,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:N6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>

</xml_diff>